<commit_message>
Update library to LSEG Data Library Update content from RDP to Workspace Update configuration file to LSEG Data Library Update README from conda to venv
</commit_message>
<xml_diff>
--- a/notebook/part2_rdp_intel_vs_amd.xlsx
+++ b/notebook/part2_rdp_intel_vs_amd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_rdlib_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA631AF-2C6E-4ADB-B155-1A2B7E446DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FFA52E-BDB2-4304-A009-BE78AEEEDFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1545" windowWidth="22710" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intel vs AMD Daily Price" sheetId="4" r:id="rId1"/>
@@ -215,21 +215,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>8022</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>188987</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>101973</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>36587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E43C3336-02C6-A2DA-A701-C7A65BDF3470}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1714DD1-8070-766F-320C-2C3C6E3AE84D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -238,7 +238,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -251,8 +251,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1790700"/>
-          <a:ext cx="10552197" cy="5522987"/>
+          <a:off x="0" y="3398520"/>
+          <a:ext cx="7363833" cy="3854207"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -263,23 +263,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>404643</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>188987</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>118893</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>173747</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22C5EA35-5C1B-C7F3-5577-37764F7C34E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{769DA5CA-26CC-5206-9305-76C3F6A1B9AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -288,7 +288,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -301,8 +301,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8401050" y="1790700"/>
-          <a:ext cx="10634493" cy="5522987"/>
+          <a:off x="8176260" y="3398422"/>
+          <a:ext cx="7685553" cy="3991465"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -326,15 +326,15 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>68602</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>188987</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>36587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFF639D-0E9B-9B67-25DC-758A99AABEAB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{800EDE9C-DC6F-50B5-48D5-EDE0EF9D1BBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -356,7 +356,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="457200"/>
+          <a:off x="0" y="449580"/>
           <a:ext cx="11041402" cy="5522987"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -382,12 +382,12 @@
   </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{84126F28-5BA5-43DA-87E1-D851FF53831B}" name="BID"/>
-    <tableColumn id="2" xr3:uid="{CE8B5C8D-B24A-413B-B228-D02EC2B2BBE8}" name="ASK"/>
-    <tableColumn id="3" xr3:uid="{F9020DD6-CE67-4503-9540-C8B47681CAD5}" name="OPEN_PRC"/>
-    <tableColumn id="4" xr3:uid="{F50F0AF2-7840-4ED9-BCC4-3B82EF27C5B3}" name="HIGH_1"/>
-    <tableColumn id="5" xr3:uid="{D5190140-D633-4580-B975-D1C94066550E}" name="LOW_1"/>
-    <tableColumn id="6" xr3:uid="{DAE66111-58AD-498C-A6CC-9098AF8CF2D7}" name="TRDPRC_1"/>
-    <tableColumn id="7" xr3:uid="{D627AA9B-85F9-44EE-BD78-95E973B96C46}" name="BLKVOLUM"/>
+    <tableColumn id="2" xr3:uid="{C4E0D353-7BB2-49A2-8C1B-660FBCE0D3BA}" name="ASK"/>
+    <tableColumn id="3" xr3:uid="{E38AB1A1-6F36-4416-AD87-6005DE6FDC2D}" name="OPEN_PRC"/>
+    <tableColumn id="4" xr3:uid="{746A2698-4FE7-48B8-A551-E70CBDC98BE2}" name="HIGH_1"/>
+    <tableColumn id="5" xr3:uid="{F6C19C06-431B-45F2-9350-99D98FFD6844}" name="LOW_1"/>
+    <tableColumn id="6" xr3:uid="{7E2D258D-999E-4186-8EE3-90D196F860FC}" name="TRDPRC_1"/>
+    <tableColumn id="7" xr3:uid="{BBCD8789-F7FC-4F26-9E88-3C1D7CAD9A21}" name="BLKVOLUM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -406,12 +406,12 @@
   </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A67C05C2-23BE-499F-A773-B002393BCD63}" name="BID"/>
-    <tableColumn id="2" xr3:uid="{99519E5D-9C3B-4383-939B-38C01DBA9CA1}" name="ASK"/>
-    <tableColumn id="3" xr3:uid="{4C01F198-9D25-4812-9A9F-080B26C38696}" name="OPEN_PRC"/>
-    <tableColumn id="4" xr3:uid="{B729C93D-B04E-4768-A76A-03FBB922AF47}" name="HIGH_1"/>
-    <tableColumn id="5" xr3:uid="{B1FE639C-2D5C-459F-AAE2-7B84FF6CF738}" name="LOW_1"/>
-    <tableColumn id="6" xr3:uid="{B409FDF5-05E5-4C01-8737-5573036E2AA5}" name="TRDPRC_1"/>
-    <tableColumn id="7" xr3:uid="{436198C8-F741-4E71-BA07-B398A1C32440}" name="BLKVOLUM"/>
+    <tableColumn id="2" xr3:uid="{17DA8B02-172F-4A8D-90A3-762BB6A1722F}" name="ASK"/>
+    <tableColumn id="3" xr3:uid="{C2BA8F21-38A3-4605-BA9F-95624FC135E9}" name="OPEN_PRC"/>
+    <tableColumn id="4" xr3:uid="{D776FDF1-3268-455A-BFC0-5B575091DCF1}" name="HIGH_1"/>
+    <tableColumn id="5" xr3:uid="{B287BB85-8A1D-431D-A8C3-16C87C2A9638}" name="LOW_1"/>
+    <tableColumn id="6" xr3:uid="{A067EA02-9EB1-4C38-BA34-8CB97F6EA92F}" name="TRDPRC_1"/>
+    <tableColumn id="7" xr3:uid="{990279B1-89C3-43AF-92E7-B26C635B4115}" name="BLKVOLUM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -682,20 +682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB8FC013-95A6-4FF9-BDAB-F9F2B6095DAD}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
     <col min="2" max="3" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="21" max="21" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -717,7 +719,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -761,661 +763,661 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>33.83</v>
+        <v>23.56</v>
       </c>
       <c r="B3">
-        <v>33.85</v>
+        <v>23.57</v>
       </c>
       <c r="C3">
-        <v>34.15</v>
+        <v>23.05</v>
       </c>
       <c r="D3">
-        <v>34.299999999999997</v>
+        <v>23.82</v>
       </c>
       <c r="E3">
-        <v>33.619999999999997</v>
+        <v>22.98</v>
       </c>
       <c r="F3">
-        <v>33.869999999999997</v>
+        <v>23.56</v>
       </c>
       <c r="G3">
-        <v>10714959</v>
+        <v>8414059</v>
       </c>
       <c r="N3">
-        <v>115.89</v>
+        <v>167.86</v>
       </c>
       <c r="O3">
-        <v>115.91</v>
+        <v>167.89</v>
       </c>
       <c r="P3">
-        <v>115.76</v>
+        <v>164.185</v>
       </c>
       <c r="Q3">
-        <v>116.16</v>
+        <v>169.35</v>
       </c>
       <c r="R3">
-        <v>113.575</v>
+        <v>163.01009999999999</v>
       </c>
       <c r="S3">
-        <v>115.92</v>
+        <v>167.89</v>
       </c>
       <c r="T3">
-        <v>4450863</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>3349230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>33.14</v>
+        <v>23.43</v>
       </c>
       <c r="B4">
-        <v>33.15</v>
+        <v>23.44</v>
       </c>
       <c r="C4">
-        <v>33.78</v>
+        <v>23.58</v>
       </c>
       <c r="D4">
-        <v>33.869999999999997</v>
+        <v>23.77</v>
       </c>
       <c r="E4">
-        <v>33</v>
+        <v>23.270099999999999</v>
       </c>
       <c r="F4">
-        <v>33.15</v>
+        <v>23.44</v>
       </c>
       <c r="G4">
-        <v>8218383</v>
+        <v>6816688</v>
       </c>
       <c r="N4">
-        <v>115.97</v>
+        <v>165.26</v>
       </c>
       <c r="O4">
-        <v>115.98</v>
+        <v>165.27</v>
       </c>
       <c r="P4">
-        <v>116.17</v>
+        <v>167.77</v>
       </c>
       <c r="Q4">
-        <v>122.12</v>
+        <v>168.9</v>
       </c>
       <c r="R4">
-        <v>115.25</v>
+        <v>165.15</v>
       </c>
       <c r="S4">
-        <v>115.94</v>
+        <v>165.27</v>
       </c>
       <c r="T4">
-        <v>4922093</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2655449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>34.36</v>
+        <v>22.68</v>
       </c>
       <c r="B5">
-        <v>34.369999999999997</v>
+        <v>22.69</v>
       </c>
       <c r="C5">
-        <v>33.159999999999997</v>
+        <v>23.41</v>
       </c>
       <c r="D5">
-        <v>34.6</v>
+        <v>23.72</v>
       </c>
       <c r="E5">
-        <v>33.07</v>
+        <v>22.47</v>
       </c>
       <c r="F5">
-        <v>34.369999999999997</v>
+        <v>22.66</v>
       </c>
       <c r="G5">
-        <v>7502714</v>
+        <v>19346165</v>
       </c>
       <c r="N5">
-        <v>118.29</v>
+        <v>156.66999999999999</v>
       </c>
       <c r="O5">
-        <v>118.3</v>
+        <v>156.68</v>
       </c>
       <c r="P5">
-        <v>115.95</v>
+        <v>163.21</v>
       </c>
       <c r="Q5">
-        <v>118.8399</v>
+        <v>164.13</v>
       </c>
       <c r="R5">
-        <v>112.73</v>
+        <v>155.74</v>
       </c>
       <c r="S5">
-        <v>118.32</v>
+        <v>156.63999999999999</v>
       </c>
       <c r="T5">
-        <v>4254126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>5209303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>34.49</v>
+        <v>22.31</v>
       </c>
       <c r="B6">
-        <v>34.5</v>
+        <v>22.32</v>
       </c>
       <c r="C6">
-        <v>34.28</v>
+        <v>22.38</v>
       </c>
       <c r="D6">
-        <v>34.700000000000003</v>
+        <v>22.54</v>
       </c>
       <c r="E6">
-        <v>33.83</v>
+        <v>21.74</v>
       </c>
       <c r="F6">
-        <v>34.5</v>
+        <v>22.31</v>
       </c>
       <c r="G6">
-        <v>6321460</v>
+        <v>11654041</v>
       </c>
       <c r="N6">
-        <v>117.9</v>
+        <v>156.1</v>
       </c>
       <c r="O6">
-        <v>117.91</v>
+        <v>156.15</v>
       </c>
       <c r="P6">
-        <v>117.55</v>
+        <v>158.07499999999999</v>
       </c>
       <c r="Q6">
-        <v>118.43</v>
+        <v>158.28</v>
       </c>
       <c r="R6">
-        <v>115.19199999999999</v>
+        <v>154.91589999999999</v>
       </c>
       <c r="S6">
-        <v>117.93</v>
+        <v>156.13</v>
       </c>
       <c r="T6">
-        <v>3687461</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1905271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>34.44</v>
+        <v>22.44</v>
       </c>
       <c r="B7">
-        <v>34.450000000000003</v>
+        <v>22.45</v>
       </c>
       <c r="C7">
-        <v>34.4</v>
+        <v>22.72</v>
       </c>
       <c r="D7">
-        <v>34.835000000000001</v>
+        <v>22.82</v>
       </c>
       <c r="E7">
-        <v>34.33</v>
+        <v>22.4</v>
       </c>
       <c r="F7">
-        <v>34.46</v>
+        <v>22.44</v>
       </c>
       <c r="G7">
-        <v>8995771</v>
+        <v>8946662</v>
       </c>
       <c r="N7">
-        <v>116.4</v>
+        <v>156.26</v>
       </c>
       <c r="O7">
-        <v>116.41</v>
+        <v>156.28</v>
       </c>
       <c r="P7">
-        <v>121.3</v>
+        <v>160</v>
       </c>
       <c r="Q7">
-        <v>121.6699</v>
+        <v>160.44</v>
       </c>
       <c r="R7">
-        <v>115.55</v>
+        <v>156.19999999999999</v>
       </c>
       <c r="S7">
-        <v>116.43</v>
+        <v>156.25</v>
       </c>
       <c r="T7">
-        <v>4227176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2572846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>33.369999999999997</v>
+        <v>22.77</v>
       </c>
       <c r="B8">
-        <v>33.380000000000003</v>
+        <v>22.78</v>
       </c>
       <c r="C8">
-        <v>33.704000000000001</v>
+        <v>22.61</v>
       </c>
       <c r="D8">
-        <v>34.204999999999998</v>
+        <v>22.82</v>
       </c>
       <c r="E8">
-        <v>33.229999999999997</v>
+        <v>22.5</v>
       </c>
       <c r="F8">
-        <v>33.369999999999997</v>
+        <v>22.77</v>
       </c>
       <c r="G8">
-        <v>11895676</v>
+        <v>16060739</v>
       </c>
       <c r="N8">
-        <v>110.26</v>
+        <v>155.93</v>
       </c>
       <c r="O8">
-        <v>110.27</v>
+        <v>155.97999999999999</v>
       </c>
       <c r="P8">
-        <v>114.96</v>
+        <v>157.41</v>
       </c>
       <c r="Q8">
-        <v>115.05</v>
+        <v>158.01</v>
       </c>
       <c r="R8">
-        <v>109.24</v>
+        <v>155.56</v>
       </c>
       <c r="S8">
-        <v>110.25</v>
+        <v>155.97</v>
       </c>
       <c r="T8">
-        <v>8126417</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>4659489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>34</v>
+        <v>22.86</v>
       </c>
       <c r="B9">
-        <v>34.01</v>
+        <v>22.87</v>
       </c>
       <c r="C9">
-        <v>33.725000000000001</v>
+        <v>22.61</v>
       </c>
       <c r="D9">
-        <v>34.25</v>
+        <v>22.88</v>
       </c>
       <c r="E9">
-        <v>33.42</v>
+        <v>22.25</v>
       </c>
       <c r="F9">
-        <v>34.020000000000003</v>
+        <v>22.84</v>
       </c>
       <c r="G9">
-        <v>51114716</v>
+        <v>12699552</v>
       </c>
       <c r="N9">
-        <v>110.9</v>
+        <v>157.94999999999999</v>
       </c>
       <c r="O9">
-        <v>110.92</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="P9">
-        <v>110.97</v>
+        <v>155.76</v>
       </c>
       <c r="Q9">
-        <v>112.3</v>
+        <v>158</v>
       </c>
       <c r="R9">
-        <v>109.54</v>
+        <v>154.15</v>
       </c>
       <c r="S9">
-        <v>110.95</v>
+        <v>157.9</v>
       </c>
       <c r="T9">
-        <v>23109961</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>3229187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B10">
-        <v>33.65</v>
+        <v>22.4</v>
       </c>
       <c r="C10">
-        <v>33.840000000000003</v>
+        <v>22.73</v>
       </c>
       <c r="D10">
-        <v>34.46</v>
+        <v>22.82</v>
       </c>
       <c r="E10">
-        <v>33.56</v>
+        <v>22.17</v>
       </c>
       <c r="F10">
-        <v>33.630000000000003</v>
+        <v>22.4</v>
       </c>
       <c r="G10">
-        <v>4584591</v>
+        <v>18769321</v>
       </c>
       <c r="M10" t="s">
         <v>1</v>
       </c>
       <c r="O10">
-        <v>110.61</v>
+        <v>154.07</v>
       </c>
       <c r="P10">
-        <v>110.617</v>
+        <v>156.6</v>
       </c>
       <c r="Q10">
-        <v>111.31</v>
+        <v>156.74</v>
       </c>
       <c r="R10">
-        <v>108.55</v>
+        <v>151.91</v>
       </c>
       <c r="S10">
-        <v>110.61</v>
+        <v>154.09</v>
       </c>
       <c r="T10">
-        <v>2999348</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+        <v>3532117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>34.08</v>
+        <v>21.98</v>
       </c>
       <c r="B11">
-        <v>34.090000000000003</v>
+        <v>21.99</v>
       </c>
       <c r="C11">
-        <v>33.700000000000003</v>
+        <v>22.3</v>
       </c>
       <c r="D11">
-        <v>34.340000000000003</v>
+        <v>22.425000000000001</v>
       </c>
       <c r="E11">
-        <v>33.4</v>
+        <v>21.574999999999999</v>
       </c>
       <c r="F11">
-        <v>34.1</v>
+        <v>21.98</v>
       </c>
       <c r="G11">
-        <v>6419374</v>
+        <v>9881082</v>
       </c>
       <c r="N11">
-        <v>113</v>
+        <v>152.91</v>
       </c>
       <c r="O11">
-        <v>113.01</v>
+        <v>152.93</v>
       </c>
       <c r="P11">
-        <v>111.14</v>
+        <v>153</v>
       </c>
       <c r="Q11">
-        <v>114.05</v>
+        <v>153.44499999999999</v>
       </c>
       <c r="R11">
-        <v>111</v>
+        <v>150.52000000000001</v>
       </c>
       <c r="S11">
-        <v>113</v>
+        <v>152.91</v>
       </c>
       <c r="T11">
-        <v>4239211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2217639</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>34.369999999999997</v>
+        <v>22.33</v>
       </c>
       <c r="B12">
-        <v>34.380000000000003</v>
+        <v>22.34</v>
       </c>
       <c r="C12">
-        <v>33.72</v>
+        <v>22.09</v>
       </c>
       <c r="D12">
-        <v>34.524999999999999</v>
+        <v>22.364999999999998</v>
       </c>
       <c r="E12">
-        <v>33.700000000000003</v>
+        <v>21.97</v>
       </c>
       <c r="F12">
-        <v>34.36</v>
+        <v>22.34</v>
       </c>
       <c r="G12">
-        <v>12010393</v>
+        <v>11829447</v>
       </c>
       <c r="N12">
-        <v>110.09</v>
+        <v>153.41999999999999</v>
       </c>
       <c r="O12">
-        <v>110.11</v>
+        <v>153.44</v>
       </c>
       <c r="P12">
-        <v>111.91</v>
+        <v>154.74</v>
       </c>
       <c r="Q12">
-        <v>112.36</v>
+        <v>155.19</v>
       </c>
       <c r="R12">
-        <v>109.3</v>
+        <v>152.35</v>
       </c>
       <c r="S12">
-        <v>110.09</v>
+        <v>153.44</v>
       </c>
       <c r="T12">
-        <v>3661789</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>3188927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>34.56</v>
+        <v>22.67</v>
       </c>
       <c r="B13">
-        <v>34.57</v>
+        <v>22.68</v>
       </c>
       <c r="C13">
-        <v>34.82</v>
+        <v>22.42</v>
       </c>
       <c r="D13">
-        <v>35.03</v>
+        <v>23.3399</v>
       </c>
       <c r="E13">
-        <v>34.11</v>
+        <v>22.41</v>
       </c>
       <c r="F13">
-        <v>34.549999999999997</v>
+        <v>22.68</v>
       </c>
       <c r="G13">
-        <v>10710747</v>
+        <v>23885891</v>
       </c>
       <c r="N13">
-        <v>111.11</v>
+        <v>156.22</v>
       </c>
       <c r="O13">
-        <v>111.12</v>
+        <v>156.28</v>
       </c>
       <c r="P13">
-        <v>111.79</v>
+        <v>155.4</v>
       </c>
       <c r="Q13">
-        <v>115.08</v>
+        <v>158.91</v>
       </c>
       <c r="R13">
-        <v>110.51</v>
+        <v>155.05000000000001</v>
       </c>
       <c r="S13">
-        <v>111.1</v>
+        <v>156.22999999999999</v>
       </c>
       <c r="T13">
-        <v>3526602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>4248523</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>36.81</v>
+        <v>22.93</v>
       </c>
       <c r="B14">
-        <v>36.82</v>
+        <v>22.94</v>
       </c>
       <c r="C14">
-        <v>36.75</v>
+        <v>22.67</v>
       </c>
       <c r="D14">
-        <v>36.99</v>
+        <v>23.27</v>
       </c>
       <c r="E14">
-        <v>35.51</v>
+        <v>22.56</v>
       </c>
       <c r="F14">
-        <v>36.83</v>
+        <v>22.92</v>
       </c>
       <c r="G14">
-        <v>14565648</v>
+        <v>12568521</v>
       </c>
       <c r="N14">
-        <v>112.95</v>
+        <v>159.87</v>
       </c>
       <c r="O14">
-        <v>112.96</v>
+        <v>159.91999999999999</v>
       </c>
       <c r="P14">
-        <v>113.38</v>
+        <v>158.5</v>
       </c>
       <c r="Q14">
-        <v>114.86</v>
+        <v>160.28</v>
       </c>
       <c r="R14">
-        <v>112.44</v>
+        <v>157.04499999999999</v>
       </c>
       <c r="S14">
-        <v>112.96</v>
+        <v>159.91999999999999</v>
       </c>
       <c r="T14">
-        <v>4630583</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>8526385</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>35.79</v>
+        <v>22.92</v>
       </c>
       <c r="B15">
-        <v>35.799999999999997</v>
+        <v>22.93</v>
       </c>
       <c r="C15">
-        <v>36.869999999999997</v>
+        <v>22.87</v>
       </c>
       <c r="D15">
-        <v>37.19</v>
+        <v>23.14</v>
       </c>
       <c r="E15">
-        <v>35.674999999999997</v>
+        <v>22.41</v>
       </c>
       <c r="F15">
-        <v>35.770000000000003</v>
+        <v>22.9</v>
       </c>
       <c r="G15">
-        <v>22021695</v>
+        <v>41750514</v>
       </c>
       <c r="N15">
-        <v>114.42</v>
+        <v>166.27</v>
       </c>
       <c r="O15">
-        <v>114.43</v>
+        <v>166.35</v>
       </c>
       <c r="P15">
-        <v>114.16</v>
+        <v>161.1</v>
       </c>
       <c r="Q15">
-        <v>114.68</v>
+        <v>167.50989999999999</v>
       </c>
       <c r="R15">
-        <v>112.35</v>
+        <v>158.94</v>
       </c>
       <c r="S15">
-        <v>114.4</v>
+        <v>166.25</v>
       </c>
       <c r="T15">
-        <v>4318272</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>8602240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>35.79</v>
+        <v>22.28</v>
       </c>
       <c r="B16">
-        <v>35.799999999999997</v>
+        <v>22.29</v>
       </c>
       <c r="C16">
-        <v>35.82</v>
+        <v>22.414999999999999</v>
       </c>
       <c r="D16">
-        <v>36.020000000000003</v>
+        <v>22.93</v>
       </c>
       <c r="E16">
-        <v>35.28</v>
+        <v>22.26</v>
       </c>
       <c r="F16">
-        <v>35.799999999999997</v>
+        <v>22.3</v>
       </c>
       <c r="G16">
-        <v>3982464</v>
+        <v>13279258</v>
       </c>
       <c r="N16">
-        <v>117.64</v>
+        <v>148.59</v>
       </c>
       <c r="O16">
-        <v>117.66</v>
+        <v>148.69999999999999</v>
       </c>
       <c r="P16">
-        <v>114.26</v>
+        <v>153.01</v>
       </c>
       <c r="Q16">
-        <v>118.19</v>
+        <v>153.12</v>
       </c>
       <c r="R16">
-        <v>113.16</v>
+        <v>148.1</v>
       </c>
       <c r="S16">
-        <v>117.6</v>
+        <v>148.6</v>
       </c>
       <c r="T16">
-        <v>4772232</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+        <v>11220758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>34.369999999999997</v>
+        <v>21.53</v>
       </c>
       <c r="B17">
-        <v>34.380000000000003</v>
+        <v>21.54</v>
       </c>
       <c r="C17">
-        <v>35.15</v>
+        <v>22.15</v>
       </c>
       <c r="D17">
-        <v>35.18</v>
+        <v>22.25</v>
       </c>
       <c r="E17">
-        <v>34.280999999999999</v>
+        <v>21.47</v>
       </c>
       <c r="F17">
-        <v>34.39</v>
+        <v>21.52</v>
       </c>
       <c r="G17">
-        <v>9684902</v>
+        <v>26895753</v>
       </c>
       <c r="N17">
-        <v>109.36</v>
+        <v>144.03</v>
       </c>
       <c r="O17">
-        <v>109.37</v>
+        <v>144.07</v>
       </c>
       <c r="P17">
-        <v>119.49</v>
+        <v>147.80000000000001</v>
       </c>
       <c r="Q17">
-        <v>119.5</v>
+        <v>148.68</v>
       </c>
       <c r="R17">
-        <v>107.38</v>
+        <v>143.33000000000001</v>
       </c>
       <c r="S17">
-        <v>109.35</v>
+        <v>144.07</v>
       </c>
       <c r="T17">
-        <v>7986689</v>
+        <v>5358151</v>
       </c>
     </row>
   </sheetData>
@@ -1435,9 +1437,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>